<commit_message>
modulo 3 - estudo de caso, projetando banco de dados sivenp
</commit_message>
<xml_diff>
--- a/codigo/2-Conceitual/0-planilha/Lista de produtos.xlsx
+++ b/codigo/2-Conceitual/0-planilha/Lista de produtos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Joab\Documentos\JOBS\Minicursos\minicurso_mysql\codigo\2-Conceitual\0-planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Joab\Documentos\JOBS\Minicursos\minicurso_mysql2\codigo\2-Conceitual\0-planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="5100"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de produtos" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +555,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="5">
-        <f>(F2-E2)*D2</f>
+        <f t="shared" ref="G2:G24" si="0">(F2-E2)*D2</f>
         <v>20</v>
       </c>
     </row>
@@ -579,7 +579,7 @@
         <v>6.5</v>
       </c>
       <c r="G3" s="5">
-        <f>(F3-E3)*D3</f>
+        <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
     </row>
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="5">
-        <f>(F4-E4)*D4</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -627,7 +627,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="5">
-        <f>(F5-E5)*D5</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
@@ -651,7 +651,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="5">
-        <f>(F6-E6)*D6</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
@@ -675,7 +675,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="5">
-        <f>(F7-E7)*D7</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -699,7 +699,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="5">
-        <f>(F8-E8)*D8</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="5">
-        <f>(F9-E9)*D9</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -747,7 +747,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="5">
-        <f>(F10-E10)*D10</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -771,7 +771,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="5">
-        <f>(F11-E11)*D11</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -795,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="5">
-        <f>(F12-E12)*D12</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="5">
-        <f>(F13-E13)*D13</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
@@ -843,7 +843,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="5">
-        <f>(F14-E14)*D14</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
@@ -867,7 +867,7 @@
         <v>9</v>
       </c>
       <c r="G15" s="5">
-        <f>(F15-E15)*D15</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
@@ -891,7 +891,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="5">
-        <f>(F16-E16)*D16</f>
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
     </row>
@@ -915,7 +915,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="5">
-        <f>(F17-E17)*D17</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -939,7 +939,7 @@
         <v>9.9</v>
       </c>
       <c r="G18" s="5">
-        <f>(F18-E18)*D18</f>
+        <f t="shared" si="0"/>
         <v>54.000000000000021</v>
       </c>
     </row>
@@ -963,7 +963,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="5">
-        <f>(F19-E19)*D19</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
@@ -987,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="5">
-        <f>(F20-E20)*D20</f>
+        <f t="shared" si="0"/>
         <v>-30</v>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="5">
-        <f>(F21-E21)*D21</f>
+        <f t="shared" si="0"/>
         <v>-84</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="5">
-        <f>(F22-E22)*D22</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="G23" s="5">
-        <f>(F23-E23)*D23</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
@@ -1083,7 +1083,7 @@
         <v>11</v>
       </c>
       <c r="G24" s="5">
-        <f>(F24-E24)*D24</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>

</xml_diff>